<commit_message>
Fix Catalog Version -  LIKE Node Name
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/60_Inst_BusinessLine_ISPRO.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/60_Inst_BusinessLine_ISPRO.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="26175" windowHeight="11400" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Business_Line" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="r Subset_AnalysisUnit" sheetId="10" r:id="rId10"/>
     <sheet name="Fields definition" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="124">
   <si>
     <t>Business_Line</t>
   </si>
@@ -474,9 +474,6 @@
     <t>FILTER_VAR_CORPORATE</t>
   </si>
   <si>
-    <t>CORPORATE</t>
-  </si>
-  <si>
     <t>CORPORATE_EQUALS</t>
   </si>
   <si>
@@ -514,6 +511,141 @@
   </si>
   <si>
     <t>COUNTERPARTY_ISPRO</t>
+  </si>
+  <si>
+    <t>BL_ISPRO_000002</t>
+  </si>
+  <si>
+    <t>SME Corporate</t>
+  </si>
+  <si>
+    <t>SME Retail</t>
+  </si>
+  <si>
+    <t>Corporate RED</t>
+  </si>
+  <si>
+    <t>SME Corporate RED</t>
+  </si>
+  <si>
+    <t>SME Retail RED</t>
+  </si>
+  <si>
+    <t>BL_ISPRO_000003</t>
+  </si>
+  <si>
+    <t>BL_ISPRO_000004</t>
+  </si>
+  <si>
+    <t>BL_ISPRO_000005</t>
+  </si>
+  <si>
+    <t>BL_ISPRO_000006</t>
+  </si>
+  <si>
+    <t>(SEGMENT='SME Corporate')</t>
+  </si>
+  <si>
+    <t>(SEGMENT='SME Retail')</t>
+  </si>
+  <si>
+    <t>(SEGMENT='Corporate RED')</t>
+  </si>
+  <si>
+    <t>(SEGMENT='SME Corporate RED')</t>
+  </si>
+  <si>
+    <t>(SEGMENT='SME Retail RED')</t>
+  </si>
+  <si>
+    <t>FI_ISPRO_0000002</t>
+  </si>
+  <si>
+    <t>FI_ISPRO_0000003</t>
+  </si>
+  <si>
+    <t>FI_ISPRO_0000004</t>
+  </si>
+  <si>
+    <t>FI_ISPRO_0000005</t>
+  </si>
+  <si>
+    <t>FI_ISPRO_0000006</t>
+  </si>
+  <si>
+    <t>FILTER_SME_Corporate</t>
+  </si>
+  <si>
+    <t>FILTER_SME_Retail</t>
+  </si>
+  <si>
+    <t>FILTER_Corporate_RED</t>
+  </si>
+  <si>
+    <t>FILTER_SME Corporate_RED</t>
+  </si>
+  <si>
+    <t>FILTER_SME Retail_RED</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_VAR_02</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_VAR_03</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_VAR_04</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_VAR_05</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_VAR_06</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_OPERATOR_02</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_OPERATOR_03</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_OPERATOR_04</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_OPERATOR_05</t>
+  </si>
+  <si>
+    <t>R_FILTER_ISPRO_OPERATOR_06</t>
+  </si>
+  <si>
+    <t>FV_ISPRO_0000002</t>
+  </si>
+  <si>
+    <t>FV_ISPRO_0000003</t>
+  </si>
+  <si>
+    <t>FV_ISPRO_0000004</t>
+  </si>
+  <si>
+    <t>FV_ISPRO_0000005</t>
+  </si>
+  <si>
+    <t>FV_ISPRO_0000006</t>
+  </si>
+  <si>
+    <t>BRAU_ISPRO_0000002</t>
+  </si>
+  <si>
+    <t>BRAU_ISPRO_0000003</t>
+  </si>
+  <si>
+    <t>BRAU_ISPRO_0000004</t>
+  </si>
+  <si>
+    <t>BRAU_ISPRO_0000005</t>
+  </si>
+  <si>
+    <t>BRAU_ISPRO_0000006</t>
   </si>
 </sst>
 </file>
@@ -573,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -581,6 +713,12 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +753,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -658,7 +802,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -706,7 +856,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -754,7 +910,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -802,7 +964,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -850,7 +1018,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -898,7 +1072,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -946,7 +1126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -994,7 +1180,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1042,7 +1234,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1090,7 +1288,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1146,7 +1350,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1202,7 +1412,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1258,7 +1474,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1306,7 +1528,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1315,6 +1543,60 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10296525" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8353425" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1359,7 +1641,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10242" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="10242" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002280000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1402,7 +1690,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1450,7 +1744,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1498,7 +1798,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1546,7 +1852,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1594,7 +1906,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1642,7 +1960,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1690,7 +2014,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1738,7 +2068,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1786,7 +2122,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1834,7 +2176,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1890,7 +2238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1946,7 +2300,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2002,7 +2362,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2050,7 +2416,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2059,6 +2431,60 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10639425" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11029950" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2103,7 +2529,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2146,7 +2578,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2194,7 +2632,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2242,7 +2686,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2290,7 +2740,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2338,7 +2794,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2386,7 +2848,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2434,7 +2902,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2482,7 +2956,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2530,7 +3010,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2578,7 +3064,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2634,7 +3126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2690,7 +3188,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2746,7 +3250,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2794,7 +3304,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2803,6 +3319,60 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9667875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9667875" cy="9515475"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2847,7 +3417,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3074" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="3074" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2890,7 +3466,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2938,7 +3520,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2986,7 +3574,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3034,7 +3628,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3082,7 +3682,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3130,7 +3736,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3178,7 +3790,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3226,7 +3844,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3274,7 +3898,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3322,7 +3952,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3378,7 +4014,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3434,7 +4076,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3490,7 +4138,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3538,7 +4192,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3591,7 +4305,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4098" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="4098" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3634,7 +4354,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3682,7 +4408,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3730,7 +4462,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3778,7 +4516,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3826,7 +4570,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3874,7 +4624,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3922,7 +4678,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3970,7 +4732,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4018,7 +4786,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4066,7 +4840,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4122,7 +4902,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4178,7 +4964,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4234,7 +5026,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4282,7 +5080,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4335,7 +5193,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5122" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="5122" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002140000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4378,7 +5242,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4426,7 +5296,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4474,7 +5350,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4522,7 +5404,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4570,7 +5458,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4618,7 +5512,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4666,7 +5566,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4714,7 +5620,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4762,7 +5674,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4810,7 +5728,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4866,7 +5790,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4922,7 +5852,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4978,7 +5914,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5026,7 +5968,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9191625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5079,7 +6081,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6146" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="6146" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002180000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5122,7 +6130,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5170,7 +6184,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5218,7 +6238,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5266,7 +6292,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5314,7 +6346,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5362,7 +6400,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5410,7 +6454,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5458,7 +6508,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5506,7 +6562,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5554,7 +6616,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5610,7 +6678,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5666,7 +6740,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5722,7 +6802,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5770,7 +6856,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5779,6 +6871,60 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10048875" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10048875" cy="9515475"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5823,7 +6969,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7170" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="7170" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000021C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5866,7 +7018,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5914,7 +7072,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5962,7 +7126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6010,7 +7180,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6058,7 +7234,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6106,7 +7288,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6154,7 +7342,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6202,7 +7396,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6250,7 +7450,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6298,7 +7504,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6354,7 +7566,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6410,7 +7628,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6466,7 +7690,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6514,7 +7744,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6567,7 +7857,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8194" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="8194" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002200000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6610,7 +7906,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6658,7 +7960,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6706,7 +8014,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6754,7 +8068,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6802,7 +8122,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6850,7 +8176,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6898,7 +8230,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6946,7 +8284,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6994,7 +8338,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7042,7 +8392,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7098,7 +8454,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7154,7 +8516,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7210,7 +8578,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7258,7 +8632,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7311,7 +8745,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9218" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="9218" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7354,7 +8794,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7402,7 +8848,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7450,7 +8902,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7498,7 +8956,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7546,7 +9010,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7594,7 +9064,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7642,7 +9118,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7690,7 +9172,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7738,7 +9226,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7786,7 +9280,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7842,7 +9342,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="AutoShape 2"/>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7898,7 +9404,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvPr id="13" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7954,7 +9466,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvPr id="14" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8002,7 +9520,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvPr id="15" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -8301,10 +9879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8312,8 +9890,8 @@
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
@@ -8347,7 +9925,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
@@ -8356,31 +9934,117 @@
         <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="6" width="19.42578125" customWidth="1"/>
+    <col min="3" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8418,19 +10082,89 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>79</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -8444,7 +10178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9275,17 +11009,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
@@ -9326,7 +11060,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -9335,9 +11069,109 @@
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8">
         <v>1</v>
       </c>
     </row>
@@ -9398,16 +11232,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" customWidth="1"/>
@@ -9448,7 +11282,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -9457,10 +11291,80 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -9472,18 +11376,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9522,19 +11425,89 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -9546,19 +11519,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9617,19 +11590,19 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -9639,6 +11612,106 @@
       </c>
       <c r="K3" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>